<commit_message>
more work on hht report
</commit_message>
<xml_diff>
--- a/data/1963-2024 HHT Homeowners_Adresses_modified.xlsx
+++ b/data/1963-2024 HHT Homeowners_Adresses_modified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-24.04\home\john\projects\ssg-thefan-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A953DD-A114-4A78-A565-8552E1D40760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2BDD82-93B2-48D7-8C79-83FF4794DD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1908" windowWidth="23040" windowHeight="13560" xr2:uid="{B5D97D05-3EDC-47CB-BC1F-7CDFD2452C40}"/>
+    <workbookView xWindow="4980" yWindow="2184" windowWidth="23040" windowHeight="15516" xr2:uid="{B5D97D05-3EDC-47CB-BC1F-7CDFD2452C40}"/>
   </bookViews>
   <sheets>
     <sheet name="1963-2024" sheetId="2" r:id="rId1"/>
@@ -3003,9 +3003,6 @@
     <t xml:space="preserve">2001 Monument Ave. – Mr. &amp; Mrs. Jack (Fran) Zehmer </t>
   </si>
   <si>
-    <t xml:space="preserve"> 2235 Monument Ave. – Mr. &amp; Mrs. William B. (Janice) Rowland, Jr.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1500 West Ave. – Mr. Sheridan Snyder </t>
   </si>
   <si>
@@ -3760,6 +3757,9 @@
       </rPr>
       <t>- Chair, [No Tour]</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2235 Monument Ave. [Rixey Court] – Mr. &amp; Mrs. William B. (Janice) Rowland, Jr.  </t>
   </si>
 </sst>
 </file>
@@ -4295,8 +4295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82ABAD3-693D-4121-82C0-FE2AABF1CFBD}">
   <dimension ref="A1:D668"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180"/>
+    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="A404" sqref="A404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4307,7 +4307,7 @@
     <row r="1" spans="1:1" ht="96.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:1" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4383,17 +4383,17 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
@@ -4413,7 +4413,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -4423,7 +4423,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4443,7 +4443,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
@@ -4463,7 +4463,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -4503,15 +4503,15 @@
     </row>
     <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="C43" t="s">
         <v>639</v>
-      </c>
-      <c r="C43" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -4519,7 +4519,7 @@
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -4542,7 +4542,7 @@
         <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
@@ -4672,15 +4672,15 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C74" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -4715,7 +4715,7 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
@@ -4760,7 +4760,7 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
@@ -4855,7 +4855,7 @@
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
@@ -4890,7 +4890,7 @@
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
@@ -4910,12 +4910,12 @@
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5015,22 +5015,22 @@
     </row>
     <row r="142" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
@@ -5050,12 +5050,12 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
@@ -5075,17 +5075,17 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
@@ -5120,12 +5120,12 @@
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
@@ -5200,7 +5200,7 @@
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
@@ -5210,7 +5210,7 @@
     </row>
     <row r="181" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5220,7 +5220,7 @@
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
@@ -5265,7 +5265,7 @@
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
@@ -5280,7 +5280,7 @@
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
@@ -5290,7 +5290,7 @@
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
@@ -5300,7 +5300,7 @@
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5315,17 +5315,17 @@
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
@@ -5405,12 +5405,12 @@
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5435,17 +5435,17 @@
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
@@ -5455,12 +5455,12 @@
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5535,7 +5535,7 @@
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
@@ -5885,7 +5885,7 @@
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
@@ -5950,12 +5950,12 @@
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="331" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5980,7 +5980,7 @@
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
@@ -6010,7 +6010,7 @@
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
@@ -6060,7 +6060,7 @@
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
@@ -6070,7 +6070,7 @@
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
@@ -6125,7 +6125,7 @@
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
@@ -6190,10 +6190,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C377" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
@@ -6201,7 +6201,7 @@
         <v>262</v>
       </c>
       <c r="C378" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -6326,7 +6326,7 @@
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="6" t="s">
-        <v>478</v>
+        <v>647</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
@@ -6366,7 +6366,7 @@
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
@@ -6401,12 +6401,12 @@
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.3">
@@ -6471,12 +6471,12 @@
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="434" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6536,12 +6536,12 @@
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="447" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6551,7 +6551,7 @@
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.3">
@@ -6576,7 +6576,7 @@
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.3">
@@ -6586,7 +6586,7 @@
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.3">
@@ -6601,12 +6601,12 @@
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="460" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6666,12 +6666,12 @@
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="473" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6711,7 +6711,7 @@
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A480" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.3">
@@ -6721,7 +6721,7 @@
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.3">
@@ -6841,12 +6841,12 @@
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A507" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.3">
@@ -6866,17 +6866,17 @@
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="513" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A513" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.3">
@@ -6901,12 +6901,12 @@
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A518" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A519" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.3">
@@ -6921,12 +6921,12 @@
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A522" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A523" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="524" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -6971,7 +6971,7 @@
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.3">
@@ -7036,12 +7036,12 @@
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A545" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A546" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.3">
@@ -7135,12 +7135,12 @@
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A564" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A565" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.3">
@@ -7215,447 +7215,447 @@
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A580" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A581" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A582" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A583" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A584" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A585" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A586" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A587" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A588" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A589" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A590" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A591" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A592" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A593" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A594" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A595" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A596" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A597" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A598" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A599" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A600" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A601" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A602" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A603" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="604" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A604" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="605" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A605" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="606" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A606" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="607" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A607" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="608" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A608" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="609" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A609" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="610" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A610" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="611" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A611" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="612" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A612" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="613" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A613" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="614" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A614" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="615" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A615" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="616" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A616" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="617" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A617" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="618" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A618" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="619" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A619" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="620" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A620" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="621" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A621" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="622" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A622" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="623" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A623" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="624" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A624" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A625" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A626" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A627" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A628" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A629" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A630" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A631" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A632" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A633" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A634" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A635" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A636" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A637" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A638" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A639" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A640" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A641" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A642" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A643" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A644" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A645" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A646" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A647" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A648" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A649" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A650" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A651" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A652" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A653" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A654" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A655" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A656" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A657" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A658" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A659" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A660" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A661" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A662" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A663" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A664" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A665" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A666" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A667" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A668" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>